<commit_message>
Fully working feedback controller. Added functions for analysing the Simulation results, including extracting the forces and comparing the analytical expressions for those forces
</commit_message>
<xml_diff>
--- a/3D_Matrices.xlsx
+++ b/3D_Matrices.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sinai\Documents\Projects\Twente\Masters\Dynamics and Control\Control Week 5 - 3D - Lior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sinai\Documents\Projects\Twente\Masters\Dynamics and Control\Control Week 5 - 3D Lior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFBC28E-0B85-4062-8829-B99FF20E69C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC26D1EB-62FD-4C07-BF8B-5B9D5C5D9C15}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F4638DB1-5C33-435E-B6A7-0A0BD168DBF6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="263">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -822,6 +822,9 @@
   <si>
     <t>qdot31*qdot32*(I_upper_xx*cos(thetaA3)^2 + I_upper_zz*sin(thetaA3)^2) - qdot32*qdot33*(I_upper_xx*cos(thetaA3)*sin(thetaA3) - I_upper_zz*cos(thetaA3)*sin(thetaA3)) - I_upper_yy*qdot31*qdot32</t>
   </si>
+  <si>
+    <t>Phi</t>
+  </si>
 </sst>
 </file>
 
@@ -1198,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A853B472-AA03-4282-A8A0-667A9BCB61B2}">
   <dimension ref="A1:AR92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1340,7 +1343,9 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>262</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -7128,113 +7133,95 @@
       <c r="H47">
         <v>6</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47">
         <v>7</v>
       </c>
-      <c r="J47" s="1">
+      <c r="M47">
         <v>8</v>
       </c>
-      <c r="K47" s="1">
+      <c r="N47">
         <v>9</v>
       </c>
-      <c r="L47">
+      <c r="O47">
         <v>10</v>
       </c>
-      <c r="M47">
+      <c r="P47">
         <v>11</v>
       </c>
-      <c r="N47">
+      <c r="Q47">
         <v>12</v>
       </c>
-      <c r="O47">
+      <c r="R47">
         <v>13</v>
       </c>
-      <c r="P47">
+      <c r="S47">
         <v>14</v>
       </c>
-      <c r="Q47">
+      <c r="T47">
         <v>15</v>
       </c>
-      <c r="R47">
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47">
         <v>16</v>
       </c>
-      <c r="S47">
+      <c r="Y47">
         <v>17</v>
       </c>
-      <c r="T47">
+      <c r="Z47">
         <v>18</v>
       </c>
-      <c r="U47" s="1">
+      <c r="AA47">
         <v>19</v>
       </c>
-      <c r="V47" s="1">
+      <c r="AB47">
         <v>20</v>
       </c>
-      <c r="W47" s="1">
+      <c r="AC47">
         <v>21</v>
       </c>
-      <c r="X47">
+      <c r="AD47">
         <v>22</v>
       </c>
-      <c r="Y47">
+      <c r="AE47">
         <v>23</v>
       </c>
-      <c r="Z47">
+      <c r="AF47">
         <v>24</v>
       </c>
-      <c r="AA47">
+      <c r="AG47" s="1"/>
+      <c r="AH47" s="1"/>
+      <c r="AI47" s="1"/>
+      <c r="AJ47">
         <v>25</v>
       </c>
-      <c r="AB47">
+      <c r="AK47">
         <v>26</v>
       </c>
-      <c r="AC47">
+      <c r="AL47">
         <v>27</v>
       </c>
-      <c r="AD47">
+      <c r="AM47">
         <v>28</v>
       </c>
-      <c r="AE47">
+      <c r="AN47">
         <v>29</v>
       </c>
-      <c r="AF47">
+      <c r="AO47">
         <v>30</v>
       </c>
-      <c r="AG47" s="1">
+      <c r="AP47">
         <v>31</v>
       </c>
-      <c r="AH47" s="1">
+      <c r="AQ47">
         <v>32</v>
       </c>
-      <c r="AI47" s="1">
+      <c r="AR47">
         <v>33</v>
-      </c>
-      <c r="AJ47">
-        <v>34</v>
-      </c>
-      <c r="AK47">
-        <v>35</v>
-      </c>
-      <c r="AL47">
-        <v>36</v>
-      </c>
-      <c r="AM47">
-        <v>37</v>
-      </c>
-      <c r="AN47">
-        <v>38</v>
-      </c>
-      <c r="AO47">
-        <v>39</v>
-      </c>
-      <c r="AP47">
-        <v>40</v>
-      </c>
-      <c r="AQ47">
-        <v>41</v>
-      </c>
-      <c r="AR47">
-        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:44" x14ac:dyDescent="0.35">
@@ -7259,15 +7246,9 @@
       <c r="H48" t="s">
         <v>10</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
       <c r="L48" t="s">
         <v>14</v>
       </c>
@@ -7295,15 +7276,9 @@
       <c r="T48" t="s">
         <v>22</v>
       </c>
-      <c r="U48" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="V48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W48" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
       <c r="X48" t="s">
         <v>26</v>
       </c>
@@ -7331,15 +7306,9 @@
       <c r="AF48" t="s">
         <v>34</v>
       </c>
-      <c r="AG48" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH48" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI48" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="AG48" s="1"/>
+      <c r="AH48" s="1"/>
+      <c r="AI48" s="1"/>
       <c r="AJ48" t="s">
         <v>38</v>
       </c>
@@ -7393,15 +7362,9 @@
       <c r="H49">
         <v>0</v>
       </c>
-      <c r="I49" s="1">
-        <v>0</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>176</v>
-      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
       <c r="L49">
         <v>0</v>
       </c>
@@ -7429,15 +7392,9 @@
       <c r="T49">
         <v>0</v>
       </c>
-      <c r="U49" s="1">
-        <v>0</v>
-      </c>
-      <c r="V49" s="1">
-        <v>0</v>
-      </c>
-      <c r="W49" s="1">
-        <v>0</v>
-      </c>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
       <c r="X49">
         <v>0</v>
       </c>
@@ -7465,15 +7422,9 @@
       <c r="AF49">
         <v>0</v>
       </c>
-      <c r="AG49" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH49" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI49" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG49" s="1"/>
+      <c r="AH49" s="1"/>
+      <c r="AI49" s="1"/>
       <c r="AJ49">
         <v>0</v>
       </c>
@@ -7527,15 +7478,9 @@
       <c r="H50">
         <v>0</v>
       </c>
-      <c r="I50" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J50" s="1">
-        <v>0</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>178</v>
-      </c>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
       <c r="L50">
         <v>0</v>
       </c>
@@ -7563,15 +7508,9 @@
       <c r="T50">
         <v>0</v>
       </c>
-      <c r="U50" s="1">
-        <v>0</v>
-      </c>
-      <c r="V50" s="1">
-        <v>0</v>
-      </c>
-      <c r="W50" s="1">
-        <v>0</v>
-      </c>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
       <c r="X50">
         <v>0</v>
       </c>
@@ -7599,15 +7538,9 @@
       <c r="AF50">
         <v>0</v>
       </c>
-      <c r="AG50" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH50" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI50" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG50" s="1"/>
+      <c r="AH50" s="1"/>
+      <c r="AI50" s="1"/>
       <c r="AJ50">
         <v>0</v>
       </c>
@@ -7661,15 +7594,9 @@
       <c r="H51">
         <v>-1</v>
       </c>
-      <c r="I51" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="K51" s="1">
-        <v>0</v>
-      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
       <c r="L51">
         <v>0</v>
       </c>
@@ -7697,15 +7624,9 @@
       <c r="T51">
         <v>0</v>
       </c>
-      <c r="U51" s="1">
-        <v>0</v>
-      </c>
-      <c r="V51" s="1">
-        <v>0</v>
-      </c>
-      <c r="W51" s="1">
-        <v>0</v>
-      </c>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
       <c r="X51">
         <v>0</v>
       </c>
@@ -7733,15 +7654,9 @@
       <c r="AF51">
         <v>0</v>
       </c>
-      <c r="AG51" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH51" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI51" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG51" s="1"/>
+      <c r="AH51" s="1"/>
+      <c r="AI51" s="1"/>
       <c r="AJ51">
         <v>0</v>
       </c>
@@ -7795,15 +7710,9 @@
       <c r="H52">
         <v>0</v>
       </c>
-      <c r="I52" s="1">
-        <v>0</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>176</v>
-      </c>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
       <c r="L52">
         <v>-1</v>
       </c>
@@ -7831,15 +7740,9 @@
       <c r="T52">
         <v>0</v>
       </c>
-      <c r="U52" s="1">
-        <v>0</v>
-      </c>
-      <c r="V52" s="1">
-        <v>0</v>
-      </c>
-      <c r="W52" s="1">
-        <v>0</v>
-      </c>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
       <c r="X52">
         <v>0</v>
       </c>
@@ -7867,15 +7770,9 @@
       <c r="AF52">
         <v>0</v>
       </c>
-      <c r="AG52" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH52" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI52" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG52" s="1"/>
+      <c r="AH52" s="1"/>
+      <c r="AI52" s="1"/>
       <c r="AJ52">
         <v>0</v>
       </c>
@@ -7929,15 +7826,9 @@
       <c r="H53">
         <v>0</v>
       </c>
-      <c r="I53" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J53" s="1">
-        <v>0</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>178</v>
-      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
       <c r="L53">
         <v>0</v>
       </c>
@@ -7965,15 +7856,9 @@
       <c r="T53">
         <v>0</v>
       </c>
-      <c r="U53" s="1">
-        <v>0</v>
-      </c>
-      <c r="V53" s="1">
-        <v>0</v>
-      </c>
-      <c r="W53" s="1">
-        <v>0</v>
-      </c>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
       <c r="X53">
         <v>0</v>
       </c>
@@ -8001,15 +7886,9 @@
       <c r="AF53">
         <v>0</v>
       </c>
-      <c r="AG53" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH53" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI53" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG53" s="1"/>
+      <c r="AH53" s="1"/>
+      <c r="AI53" s="1"/>
       <c r="AJ53">
         <v>0</v>
       </c>
@@ -8063,15 +7942,9 @@
       <c r="H54">
         <v>1</v>
       </c>
-      <c r="I54" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="K54" s="1">
-        <v>0</v>
-      </c>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
       <c r="L54">
         <v>0</v>
       </c>
@@ -8099,15 +7972,9 @@
       <c r="T54">
         <v>0</v>
       </c>
-      <c r="U54" s="1">
-        <v>0</v>
-      </c>
-      <c r="V54" s="1">
-        <v>0</v>
-      </c>
-      <c r="W54" s="1">
-        <v>0</v>
-      </c>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
       <c r="X54">
         <v>0</v>
       </c>
@@ -8135,15 +8002,9 @@
       <c r="AF54">
         <v>0</v>
       </c>
-      <c r="AG54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI54" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG54" s="1"/>
+      <c r="AH54" s="1"/>
+      <c r="AI54" s="1"/>
       <c r="AJ54">
         <v>0</v>
       </c>
@@ -8197,15 +8058,9 @@
       <c r="H55">
         <v>0</v>
       </c>
-      <c r="I55" s="1">
-        <v>0</v>
-      </c>
-      <c r="J55" s="1">
-        <v>0</v>
-      </c>
-      <c r="K55" s="1">
-        <v>0</v>
-      </c>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
       <c r="L55">
         <v>1</v>
       </c>
@@ -8233,15 +8088,9 @@
       <c r="T55">
         <v>0</v>
       </c>
-      <c r="U55" s="1">
-        <v>0</v>
-      </c>
-      <c r="V55" s="1">
-        <v>0</v>
-      </c>
-      <c r="W55" s="1">
-        <v>0</v>
-      </c>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
       <c r="X55">
         <v>0</v>
       </c>
@@ -8269,15 +8118,9 @@
       <c r="AF55">
         <v>0</v>
       </c>
-      <c r="AG55" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH55" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI55" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG55" s="1"/>
+      <c r="AH55" s="1"/>
+      <c r="AI55" s="1"/>
       <c r="AJ55">
         <v>0</v>
       </c>
@@ -8331,15 +8174,9 @@
       <c r="H56">
         <v>0</v>
       </c>
-      <c r="I56" s="1">
-        <v>0</v>
-      </c>
-      <c r="J56" s="1">
-        <v>0</v>
-      </c>
-      <c r="K56" s="1">
-        <v>0</v>
-      </c>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
       <c r="L56">
         <v>0</v>
       </c>
@@ -8367,15 +8204,9 @@
       <c r="T56">
         <v>0</v>
       </c>
-      <c r="U56" s="1">
-        <v>0</v>
-      </c>
-      <c r="V56" s="1">
-        <v>0</v>
-      </c>
-      <c r="W56" s="1">
-        <v>0</v>
-      </c>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
       <c r="X56">
         <v>0</v>
       </c>
@@ -8403,15 +8234,9 @@
       <c r="AF56">
         <v>0</v>
       </c>
-      <c r="AG56" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH56" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI56" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG56" s="1"/>
+      <c r="AH56" s="1"/>
+      <c r="AI56" s="1"/>
       <c r="AJ56">
         <v>0</v>
       </c>
@@ -8465,15 +8290,9 @@
       <c r="H57">
         <v>0</v>
       </c>
-      <c r="I57" s="1">
-        <v>0</v>
-      </c>
-      <c r="J57" s="1">
-        <v>0</v>
-      </c>
-      <c r="K57" s="1">
-        <v>0</v>
-      </c>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
       <c r="L57">
         <v>0</v>
       </c>
@@ -8501,15 +8320,9 @@
       <c r="T57">
         <v>0</v>
       </c>
-      <c r="U57" s="1">
-        <v>0</v>
-      </c>
-      <c r="V57" s="1">
-        <v>0</v>
-      </c>
-      <c r="W57" s="1">
-        <v>0</v>
-      </c>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
       <c r="X57">
         <v>0</v>
       </c>
@@ -8537,15 +8350,9 @@
       <c r="AF57">
         <v>0</v>
       </c>
-      <c r="AG57" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH57" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI57" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG57" s="1"/>
+      <c r="AH57" s="1"/>
+      <c r="AI57" s="1"/>
       <c r="AJ57">
         <v>0</v>
       </c>
@@ -8599,15 +8406,9 @@
       <c r="H58">
         <v>0</v>
       </c>
-      <c r="I58" s="1">
-        <v>0</v>
-      </c>
-      <c r="J58" s="1">
-        <v>0</v>
-      </c>
-      <c r="K58" s="1">
-        <v>0</v>
-      </c>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
       <c r="L58">
         <v>0</v>
       </c>
@@ -8635,15 +8436,9 @@
       <c r="T58">
         <v>0</v>
       </c>
-      <c r="U58" s="1">
-        <v>0</v>
-      </c>
-      <c r="V58" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="W58" s="1" t="s">
-        <v>182</v>
-      </c>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
       <c r="X58">
         <v>0</v>
       </c>
@@ -8671,15 +8466,9 @@
       <c r="AF58">
         <v>0</v>
       </c>
-      <c r="AG58" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH58" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI58" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG58" s="1"/>
+      <c r="AH58" s="1"/>
+      <c r="AI58" s="1"/>
       <c r="AJ58">
         <v>0</v>
       </c>
@@ -8733,15 +8522,9 @@
       <c r="H59">
         <v>0</v>
       </c>
-      <c r="I59" s="1">
-        <v>0</v>
-      </c>
-      <c r="J59" s="1">
-        <v>0</v>
-      </c>
-      <c r="K59" s="1">
-        <v>0</v>
-      </c>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
       <c r="L59">
         <v>0</v>
       </c>
@@ -8769,15 +8552,9 @@
       <c r="T59">
         <v>0</v>
       </c>
-      <c r="U59" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="V59" s="1">
-        <v>0</v>
-      </c>
-      <c r="W59" s="1" t="s">
-        <v>184</v>
-      </c>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
       <c r="X59">
         <v>0</v>
       </c>
@@ -8805,15 +8582,9 @@
       <c r="AF59">
         <v>0</v>
       </c>
-      <c r="AG59" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH59" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI59" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG59" s="1"/>
+      <c r="AH59" s="1"/>
+      <c r="AI59" s="1"/>
       <c r="AJ59">
         <v>0</v>
       </c>
@@ -8867,15 +8638,9 @@
       <c r="H60">
         <v>0</v>
       </c>
-      <c r="I60" s="1">
-        <v>0</v>
-      </c>
-      <c r="J60" s="1">
-        <v>0</v>
-      </c>
-      <c r="K60" s="1">
-        <v>0</v>
-      </c>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
       <c r="L60">
         <v>0</v>
       </c>
@@ -8903,15 +8668,9 @@
       <c r="T60">
         <v>-1</v>
       </c>
-      <c r="U60" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="V60" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="W60" s="1">
-        <v>0</v>
-      </c>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
       <c r="X60">
         <v>0</v>
       </c>
@@ -8939,15 +8698,9 @@
       <c r="AF60">
         <v>0</v>
       </c>
-      <c r="AG60" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH60" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI60" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG60" s="1"/>
+      <c r="AH60" s="1"/>
+      <c r="AI60" s="1"/>
       <c r="AJ60">
         <v>0</v>
       </c>
@@ -9001,15 +8754,9 @@
       <c r="H61">
         <v>0</v>
       </c>
-      <c r="I61" s="1">
-        <v>0</v>
-      </c>
-      <c r="J61" s="1">
-        <v>0</v>
-      </c>
-      <c r="K61" s="1">
-        <v>0</v>
-      </c>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
       <c r="L61">
         <v>0</v>
       </c>
@@ -9037,15 +8784,9 @@
       <c r="T61">
         <v>0</v>
       </c>
-      <c r="U61" s="1">
-        <v>0</v>
-      </c>
-      <c r="V61" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="W61" s="1" t="s">
-        <v>182</v>
-      </c>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
       <c r="X61">
         <v>-1</v>
       </c>
@@ -9073,15 +8814,9 @@
       <c r="AF61">
         <v>0</v>
       </c>
-      <c r="AG61" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH61" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI61" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG61" s="1"/>
+      <c r="AH61" s="1"/>
+      <c r="AI61" s="1"/>
       <c r="AJ61">
         <v>0</v>
       </c>
@@ -9135,15 +8870,9 @@
       <c r="H62">
         <v>0</v>
       </c>
-      <c r="I62" s="1">
-        <v>0</v>
-      </c>
-      <c r="J62" s="1">
-        <v>0</v>
-      </c>
-      <c r="K62" s="1">
-        <v>0</v>
-      </c>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
       <c r="L62">
         <v>0</v>
       </c>
@@ -9171,15 +8900,9 @@
       <c r="T62">
         <v>0</v>
       </c>
-      <c r="U62" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="V62" s="1">
-        <v>0</v>
-      </c>
-      <c r="W62" s="1" t="s">
-        <v>184</v>
-      </c>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
       <c r="X62">
         <v>0</v>
       </c>
@@ -9207,15 +8930,9 @@
       <c r="AF62">
         <v>0</v>
       </c>
-      <c r="AG62" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH62" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI62" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG62" s="1"/>
+      <c r="AH62" s="1"/>
+      <c r="AI62" s="1"/>
       <c r="AJ62">
         <v>0</v>
       </c>
@@ -9269,15 +8986,9 @@
       <c r="H63">
         <v>0</v>
       </c>
-      <c r="I63" s="1">
-        <v>0</v>
-      </c>
-      <c r="J63" s="1">
-        <v>0</v>
-      </c>
-      <c r="K63" s="1">
-        <v>0</v>
-      </c>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
       <c r="L63">
         <v>0</v>
       </c>
@@ -9305,15 +9016,9 @@
       <c r="T63">
         <v>1</v>
       </c>
-      <c r="U63" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="V63" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="W63" s="1">
-        <v>0</v>
-      </c>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
       <c r="X63">
         <v>0</v>
       </c>
@@ -9341,15 +9046,9 @@
       <c r="AF63">
         <v>0</v>
       </c>
-      <c r="AG63" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH63" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI63" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG63" s="1"/>
+      <c r="AH63" s="1"/>
+      <c r="AI63" s="1"/>
       <c r="AJ63">
         <v>0</v>
       </c>
@@ -9403,15 +9102,9 @@
       <c r="H64">
         <v>0</v>
       </c>
-      <c r="I64" s="1">
-        <v>0</v>
-      </c>
-      <c r="J64" s="1">
-        <v>0</v>
-      </c>
-      <c r="K64" s="1">
-        <v>0</v>
-      </c>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
       <c r="L64">
         <v>0</v>
       </c>
@@ -9439,15 +9132,9 @@
       <c r="T64">
         <v>0</v>
       </c>
-      <c r="U64" s="1">
-        <v>0</v>
-      </c>
-      <c r="V64" s="1">
-        <v>0</v>
-      </c>
-      <c r="W64" s="1">
-        <v>0</v>
-      </c>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
       <c r="X64">
         <v>1</v>
       </c>
@@ -9475,15 +9162,9 @@
       <c r="AF64">
         <v>0</v>
       </c>
-      <c r="AG64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI64" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG64" s="1"/>
+      <c r="AH64" s="1"/>
+      <c r="AI64" s="1"/>
       <c r="AJ64">
         <v>0</v>
       </c>
@@ -9537,15 +9218,9 @@
       <c r="H65">
         <v>0</v>
       </c>
-      <c r="I65" s="1">
-        <v>0</v>
-      </c>
-      <c r="J65" s="1">
-        <v>0</v>
-      </c>
-      <c r="K65" s="1">
-        <v>0</v>
-      </c>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
       <c r="L65">
         <v>0</v>
       </c>
@@ -9573,15 +9248,9 @@
       <c r="T65">
         <v>0</v>
       </c>
-      <c r="U65" s="1">
-        <v>0</v>
-      </c>
-      <c r="V65" s="1">
-        <v>0</v>
-      </c>
-      <c r="W65" s="1">
-        <v>0</v>
-      </c>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
       <c r="X65">
         <v>0</v>
       </c>
@@ -9609,15 +9278,9 @@
       <c r="AF65">
         <v>0</v>
       </c>
-      <c r="AG65" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH65" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI65" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG65" s="1"/>
+      <c r="AH65" s="1"/>
+      <c r="AI65" s="1"/>
       <c r="AJ65">
         <v>0</v>
       </c>
@@ -9671,15 +9334,9 @@
       <c r="H66">
         <v>0</v>
       </c>
-      <c r="I66" s="1">
-        <v>0</v>
-      </c>
-      <c r="J66" s="1">
-        <v>0</v>
-      </c>
-      <c r="K66" s="1">
-        <v>0</v>
-      </c>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
       <c r="L66">
         <v>0</v>
       </c>
@@ -9707,15 +9364,9 @@
       <c r="T66">
         <v>0</v>
       </c>
-      <c r="U66" s="1">
-        <v>0</v>
-      </c>
-      <c r="V66" s="1">
-        <v>0</v>
-      </c>
-      <c r="W66" s="1">
-        <v>0</v>
-      </c>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
       <c r="X66">
         <v>0</v>
       </c>
@@ -9743,15 +9394,9 @@
       <c r="AF66">
         <v>0</v>
       </c>
-      <c r="AG66" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH66" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI66" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG66" s="1"/>
+      <c r="AH66" s="1"/>
+      <c r="AI66" s="1"/>
       <c r="AJ66">
         <v>0</v>
       </c>
@@ -9805,15 +9450,9 @@
       <c r="H67">
         <v>0</v>
       </c>
-      <c r="I67" s="1">
-        <v>0</v>
-      </c>
-      <c r="J67" s="1">
-        <v>0</v>
-      </c>
-      <c r="K67" s="1">
-        <v>0</v>
-      </c>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
       <c r="L67">
         <v>0</v>
       </c>
@@ -9841,15 +9480,9 @@
       <c r="T67">
         <v>0</v>
       </c>
-      <c r="U67" s="1">
-        <v>0</v>
-      </c>
-      <c r="V67" s="1">
-        <v>0</v>
-      </c>
-      <c r="W67" s="1">
-        <v>0</v>
-      </c>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
       <c r="X67">
         <v>0</v>
       </c>
@@ -9877,15 +9510,9 @@
       <c r="AF67">
         <v>0</v>
       </c>
-      <c r="AG67" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH67" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AI67" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG67" s="1"/>
+      <c r="AH67" s="1"/>
+      <c r="AI67" s="1"/>
       <c r="AJ67">
         <v>0</v>
       </c>
@@ -9939,15 +9566,9 @@
       <c r="H68">
         <v>0</v>
       </c>
-      <c r="I68" s="1">
-        <v>0</v>
-      </c>
-      <c r="J68" s="1">
-        <v>0</v>
-      </c>
-      <c r="K68" s="1">
-        <v>0</v>
-      </c>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
       <c r="L68">
         <v>0</v>
       </c>
@@ -9975,15 +9596,9 @@
       <c r="T68">
         <v>0</v>
       </c>
-      <c r="U68" s="1">
-        <v>0</v>
-      </c>
-      <c r="V68" s="1">
-        <v>0</v>
-      </c>
-      <c r="W68" s="1">
-        <v>0</v>
-      </c>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
       <c r="X68">
         <v>0</v>
       </c>
@@ -10011,15 +9626,9 @@
       <c r="AF68">
         <v>0</v>
       </c>
-      <c r="AG68" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AH68" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI68" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="AG68" s="1"/>
+      <c r="AH68" s="1"/>
+      <c r="AI68" s="1"/>
       <c r="AJ68">
         <v>0</v>
       </c>
@@ -10073,15 +9682,9 @@
       <c r="H69">
         <v>0</v>
       </c>
-      <c r="I69" s="1">
-        <v>0</v>
-      </c>
-      <c r="J69" s="1">
-        <v>0</v>
-      </c>
-      <c r="K69" s="1">
-        <v>0</v>
-      </c>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
       <c r="L69">
         <v>0</v>
       </c>
@@ -10109,15 +9712,9 @@
       <c r="T69">
         <v>0</v>
       </c>
-      <c r="U69" s="1">
-        <v>0</v>
-      </c>
-      <c r="V69" s="1">
-        <v>0</v>
-      </c>
-      <c r="W69" s="1">
-        <v>0</v>
-      </c>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
       <c r="X69">
         <v>0</v>
       </c>
@@ -10145,15 +9742,9 @@
       <c r="AF69">
         <v>-1</v>
       </c>
-      <c r="AG69" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH69" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AI69" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG69" s="1"/>
+      <c r="AH69" s="1"/>
+      <c r="AI69" s="1"/>
       <c r="AJ69">
         <v>0</v>
       </c>
@@ -10207,15 +9798,9 @@
       <c r="H70">
         <v>0</v>
       </c>
-      <c r="I70" s="1">
-        <v>0</v>
-      </c>
-      <c r="J70" s="1">
-        <v>0</v>
-      </c>
-      <c r="K70" s="1">
-        <v>0</v>
-      </c>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
       <c r="L70">
         <v>0</v>
       </c>
@@ -10243,15 +9828,9 @@
       <c r="T70">
         <v>0</v>
       </c>
-      <c r="U70" s="1">
-        <v>0</v>
-      </c>
-      <c r="V70" s="1">
-        <v>0</v>
-      </c>
-      <c r="W70" s="1">
-        <v>0</v>
-      </c>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
       <c r="X70">
         <v>0</v>
       </c>
@@ -10279,15 +9858,9 @@
       <c r="AF70">
         <v>0</v>
       </c>
-      <c r="AG70" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH70" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AI70" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG70" s="1"/>
+      <c r="AH70" s="1"/>
+      <c r="AI70" s="1"/>
       <c r="AJ70">
         <v>-1</v>
       </c>
@@ -10341,15 +9914,9 @@
       <c r="H71">
         <v>0</v>
       </c>
-      <c r="I71" s="1">
-        <v>0</v>
-      </c>
-      <c r="J71" s="1">
-        <v>0</v>
-      </c>
-      <c r="K71" s="1">
-        <v>0</v>
-      </c>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
       <c r="L71">
         <v>0</v>
       </c>
@@ -10377,15 +9944,9 @@
       <c r="T71">
         <v>0</v>
       </c>
-      <c r="U71" s="1">
-        <v>0</v>
-      </c>
-      <c r="V71" s="1">
-        <v>0</v>
-      </c>
-      <c r="W71" s="1">
-        <v>0</v>
-      </c>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
       <c r="X71">
         <v>0</v>
       </c>
@@ -10413,15 +9974,9 @@
       <c r="AF71">
         <v>0</v>
       </c>
-      <c r="AG71" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AH71" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI71" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="AG71" s="1"/>
+      <c r="AH71" s="1"/>
+      <c r="AI71" s="1"/>
       <c r="AJ71">
         <v>0</v>
       </c>
@@ -10475,15 +10030,9 @@
       <c r="H72">
         <v>0</v>
       </c>
-      <c r="I72" s="1">
-        <v>0</v>
-      </c>
-      <c r="J72" s="1">
-        <v>0</v>
-      </c>
-      <c r="K72" s="1">
-        <v>0</v>
-      </c>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
       <c r="L72">
         <v>0</v>
       </c>
@@ -10511,15 +10060,9 @@
       <c r="T72">
         <v>0</v>
       </c>
-      <c r="U72" s="1">
-        <v>0</v>
-      </c>
-      <c r="V72" s="1">
-        <v>0</v>
-      </c>
-      <c r="W72" s="1">
-        <v>0</v>
-      </c>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
       <c r="X72">
         <v>0</v>
       </c>
@@ -10547,15 +10090,9 @@
       <c r="AF72">
         <v>1</v>
       </c>
-      <c r="AG72" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH72" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AI72" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG72" s="1"/>
+      <c r="AH72" s="1"/>
+      <c r="AI72" s="1"/>
       <c r="AJ72">
         <v>0</v>
       </c>
@@ -10609,15 +10146,9 @@
       <c r="H73">
         <v>0</v>
       </c>
-      <c r="I73" s="1">
-        <v>0</v>
-      </c>
-      <c r="J73" s="1">
-        <v>0</v>
-      </c>
-      <c r="K73" s="1">
-        <v>0</v>
-      </c>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
       <c r="L73">
         <v>0</v>
       </c>
@@ -10645,15 +10176,9 @@
       <c r="T73">
         <v>0</v>
       </c>
-      <c r="U73" s="1">
-        <v>0</v>
-      </c>
-      <c r="V73" s="1">
-        <v>0</v>
-      </c>
-      <c r="W73" s="1">
-        <v>0</v>
-      </c>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
       <c r="X73">
         <v>0</v>
       </c>
@@ -10681,15 +10206,9 @@
       <c r="AF73">
         <v>0</v>
       </c>
-      <c r="AG73" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH73" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI73" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG73" s="1"/>
+      <c r="AH73" s="1"/>
+      <c r="AI73" s="1"/>
       <c r="AJ73">
         <v>1</v>
       </c>
@@ -10743,15 +10262,9 @@
       <c r="H74">
         <v>0</v>
       </c>
-      <c r="I74" s="1">
-        <v>0</v>
-      </c>
-      <c r="J74" s="1">
-        <v>0</v>
-      </c>
-      <c r="K74" s="1">
-        <v>0</v>
-      </c>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
       <c r="L74">
         <v>0</v>
       </c>
@@ -10779,15 +10292,9 @@
       <c r="T74">
         <v>0</v>
       </c>
-      <c r="U74" s="1">
-        <v>0</v>
-      </c>
-      <c r="V74" s="1">
-        <v>0</v>
-      </c>
-      <c r="W74" s="1">
-        <v>0</v>
-      </c>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
       <c r="X74">
         <v>0</v>
       </c>
@@ -10815,15 +10322,9 @@
       <c r="AF74">
         <v>0</v>
       </c>
-      <c r="AG74" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH74" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI74" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG74" s="1"/>
+      <c r="AH74" s="1"/>
+      <c r="AI74" s="1"/>
       <c r="AJ74">
         <v>0</v>
       </c>
@@ -10877,15 +10378,9 @@
       <c r="H75">
         <v>0</v>
       </c>
-      <c r="I75" s="1">
-        <v>0</v>
-      </c>
-      <c r="J75" s="1">
-        <v>0</v>
-      </c>
-      <c r="K75" s="1">
-        <v>0</v>
-      </c>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
       <c r="L75">
         <v>0</v>
       </c>
@@ -10913,15 +10408,9 @@
       <c r="T75">
         <v>0</v>
       </c>
-      <c r="U75" s="1">
-        <v>0</v>
-      </c>
-      <c r="V75" s="1">
-        <v>0</v>
-      </c>
-      <c r="W75" s="1">
-        <v>0</v>
-      </c>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
       <c r="X75">
         <v>0</v>
       </c>
@@ -10949,15 +10438,9 @@
       <c r="AF75">
         <v>0</v>
       </c>
-      <c r="AG75" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH75" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI75" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG75" s="1"/>
+      <c r="AH75" s="1"/>
+      <c r="AI75" s="1"/>
       <c r="AJ75">
         <v>0</v>
       </c>
@@ -11011,15 +10494,9 @@
       <c r="H76">
         <v>0</v>
       </c>
-      <c r="I76" s="1">
-        <v>0</v>
-      </c>
-      <c r="J76" s="1">
-        <v>0</v>
-      </c>
-      <c r="K76" s="1">
-        <v>0</v>
-      </c>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
       <c r="L76">
         <v>0</v>
       </c>
@@ -11047,15 +10524,9 @@
       <c r="T76">
         <v>0</v>
       </c>
-      <c r="U76" s="1">
-        <v>0</v>
-      </c>
-      <c r="V76" s="1">
-        <v>0</v>
-      </c>
-      <c r="W76" s="1">
-        <v>0</v>
-      </c>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
       <c r="X76">
         <v>0</v>
       </c>
@@ -11083,15 +10554,9 @@
       <c r="AF76">
         <v>0</v>
       </c>
-      <c r="AG76" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH76" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI76" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG76" s="1"/>
+      <c r="AH76" s="1"/>
+      <c r="AI76" s="1"/>
       <c r="AJ76">
         <v>0</v>
       </c>
@@ -11145,15 +10610,9 @@
       <c r="H77">
         <v>0</v>
       </c>
-      <c r="I77" s="1">
-        <v>0</v>
-      </c>
-      <c r="J77" s="1">
-        <v>0</v>
-      </c>
-      <c r="K77" s="1">
-        <v>0</v>
-      </c>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
       <c r="L77">
         <v>0</v>
       </c>
@@ -11181,15 +10640,9 @@
       <c r="T77">
         <v>0</v>
       </c>
-      <c r="U77" s="1">
-        <v>0</v>
-      </c>
-      <c r="V77" s="1">
-        <v>0</v>
-      </c>
-      <c r="W77" s="1">
-        <v>0</v>
-      </c>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
       <c r="X77">
         <v>0</v>
       </c>
@@ -11217,15 +10670,9 @@
       <c r="AF77">
         <v>0</v>
       </c>
-      <c r="AG77" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH77" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI77" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG77" s="1"/>
+      <c r="AH77" s="1"/>
+      <c r="AI77" s="1"/>
       <c r="AJ77">
         <v>0</v>
       </c>
@@ -11279,15 +10726,9 @@
       <c r="H78">
         <v>0</v>
       </c>
-      <c r="I78" s="1">
-        <v>0</v>
-      </c>
-      <c r="J78" s="1">
-        <v>0</v>
-      </c>
-      <c r="K78" s="1">
-        <v>0</v>
-      </c>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
       <c r="L78">
         <v>0</v>
       </c>
@@ -11315,15 +10756,9 @@
       <c r="T78">
         <v>0</v>
       </c>
-      <c r="U78" s="1">
-        <v>0</v>
-      </c>
-      <c r="V78" s="1">
-        <v>0</v>
-      </c>
-      <c r="W78" s="1">
-        <v>0</v>
-      </c>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
       <c r="X78">
         <v>0</v>
       </c>
@@ -11351,15 +10786,9 @@
       <c r="AF78">
         <v>0</v>
       </c>
-      <c r="AG78" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH78" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI78" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG78" s="1"/>
+      <c r="AH78" s="1"/>
+      <c r="AI78" s="1"/>
       <c r="AJ78">
         <v>0</v>
       </c>
@@ -11413,15 +10842,9 @@
       <c r="H79">
         <v>0</v>
       </c>
-      <c r="I79" s="1">
-        <v>0</v>
-      </c>
-      <c r="J79" s="1">
-        <v>0</v>
-      </c>
-      <c r="K79" s="1">
-        <v>0</v>
-      </c>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
       <c r="L79">
         <v>0</v>
       </c>
@@ -11449,15 +10872,9 @@
       <c r="T79">
         <v>0</v>
       </c>
-      <c r="U79" s="1">
-        <v>0</v>
-      </c>
-      <c r="V79" s="1">
-        <v>0</v>
-      </c>
-      <c r="W79" s="1">
-        <v>0</v>
-      </c>
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+      <c r="W79" s="1"/>
       <c r="X79">
         <v>0</v>
       </c>
@@ -11485,15 +10902,9 @@
       <c r="AF79">
         <v>0</v>
       </c>
-      <c r="AG79" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH79" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI79" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG79" s="1"/>
+      <c r="AH79" s="1"/>
+      <c r="AI79" s="1"/>
       <c r="AJ79">
         <v>0</v>
       </c>
@@ -11547,15 +10958,9 @@
       <c r="H80">
         <v>0</v>
       </c>
-      <c r="I80" s="1">
-        <v>0</v>
-      </c>
-      <c r="J80" s="1">
-        <v>0</v>
-      </c>
-      <c r="K80" s="1">
-        <v>0</v>
-      </c>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
       <c r="L80">
         <v>0</v>
       </c>
@@ -11583,15 +10988,9 @@
       <c r="T80">
         <v>0</v>
       </c>
-      <c r="U80" s="1">
-        <v>0</v>
-      </c>
-      <c r="V80" s="1">
-        <v>0</v>
-      </c>
-      <c r="W80" s="1">
-        <v>0</v>
-      </c>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
       <c r="X80">
         <v>0</v>
       </c>
@@ -11619,15 +11018,9 @@
       <c r="AF80">
         <v>0</v>
       </c>
-      <c r="AG80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI80" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG80" s="1"/>
+      <c r="AH80" s="1"/>
+      <c r="AI80" s="1"/>
       <c r="AJ80">
         <v>0</v>
       </c>
@@ -11681,15 +11074,9 @@
       <c r="H81">
         <v>0</v>
       </c>
-      <c r="I81" s="1">
-        <v>0</v>
-      </c>
-      <c r="J81" s="1">
-        <v>0</v>
-      </c>
-      <c r="K81" s="1">
-        <v>0</v>
-      </c>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
       <c r="L81">
         <v>0</v>
       </c>
@@ -11717,15 +11104,9 @@
       <c r="T81">
         <v>0</v>
       </c>
-      <c r="U81" s="1">
-        <v>0</v>
-      </c>
-      <c r="V81" s="1">
-        <v>0</v>
-      </c>
-      <c r="W81" s="1">
-        <v>0</v>
-      </c>
+      <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+      <c r="W81" s="1"/>
       <c r="X81">
         <v>0</v>
       </c>
@@ -11753,15 +11134,9 @@
       <c r="AF81">
         <v>0</v>
       </c>
-      <c r="AG81" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH81" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI81" s="1">
-        <v>0</v>
-      </c>
+      <c r="AG81" s="1"/>
+      <c r="AH81" s="1"/>
+      <c r="AI81" s="1"/>
       <c r="AJ81">
         <v>0</v>
       </c>

</xml_diff>